<commit_message>
ExternalReferences changed to Links in Excel sheet
</commit_message>
<xml_diff>
--- a/test_files/Code_list_with_links_invalid_propertytype.xlsx
+++ b/test_files/Code_list_with_links_invalid_propertytype.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="CodeSchemes" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="ExternalReferences_200" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Links_200" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Codes_200" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="Extensions_200" sheetId="4" r:id="rId6"/>
   </sheets>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="179">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -22,538 +22,535 @@
     <t>ORGANIZATION</t>
   </si>
   <si>
+    <t>BROADER</t>
+  </si>
+  <si>
     <t>INFORMATIONDOMAIN</t>
   </si>
   <si>
+    <t>STATUS</t>
+  </si>
+  <si>
     <t>LANGUAGECODE</t>
   </si>
   <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
     <t>VERSION</t>
   </si>
   <si>
-    <t>STATUS</t>
+    <t>HREF</t>
+  </si>
+  <si>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
+    <t>CONCEPTURI</t>
   </si>
   <si>
     <t>SOURCE</t>
   </si>
   <si>
+    <t>HIERARCHYLEVEL</t>
+  </si>
+  <si>
+    <t>PROPERTYTYPE</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>TITLE_FI</t>
+  </si>
+  <si>
     <t>LEGALBASE</t>
   </si>
   <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>TITLE_SV</t>
+  </si>
+  <si>
     <t>GOVERNANCEPOLICY</t>
   </si>
   <si>
-    <t>CONCEPTURI</t>
+    <t>TITLE_EN</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_FI</t>
   </si>
   <si>
     <t>DEFAULTCODE</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>CREATED</t>
   </si>
   <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
     <t>MODIFIED</t>
   </si>
   <si>
-    <t>HREF</t>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>testcode28</t>
+  </si>
+  <si>
+    <t>https://lähde.fi</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>CODESSHEET</t>
   </si>
   <si>
-    <t>EXTERNALREFERENCESSHEET</t>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
+    <t>Lähde</t>
+  </si>
+  <si>
+    <t>Testcode 28</t>
+  </si>
+  <si>
+    <t>LINKSSHEET</t>
+  </si>
+  <si>
+    <t>lähde.com</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>uusi lähde</t>
+  </si>
+  <si>
+    <t>2018-11-08 11:48:30</t>
+  </si>
+  <si>
+    <t>lisenssi.fi</t>
+  </si>
+  <si>
+    <t>2018-11-08 12:01:43</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>lähde.com|lisenssi.fi|käyttöohje.fi|linkki.fi</t>
+  </si>
+  <si>
+    <t>uusi lisenssi</t>
+  </si>
+  <si>
+    <t>testcode29</t>
+  </si>
+  <si>
+    <t>test.fi</t>
+  </si>
+  <si>
+    <t>isRequiredBy</t>
+  </si>
+  <si>
+    <t>käyttöedellytys</t>
+  </si>
+  <si>
+    <t>Testcode 29</t>
+  </si>
+  <si>
+    <t>https://www.suomi.fi/etusivu/</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>lähde.com|lisenssi.fi</t>
+  </si>
+  <si>
+    <t>isReferencedBy</t>
+  </si>
+  <si>
+    <t>käyttökohde</t>
+  </si>
+  <si>
+    <t>testcode30</t>
+  </si>
+  <si>
+    <t>standardi.fi</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>Testcode 30</t>
+  </si>
+  <si>
+    <t>Liittyvä standardi</t>
   </si>
   <si>
     <t>EXTENSIONSSHEET</t>
   </si>
   <si>
+    <t>testikäyttöohje.fi</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Käyttöohje</t>
+  </si>
+  <si>
     <t>74a41211-8c99-4835-a519-7a61612b1098</t>
   </si>
   <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
     <t>P1</t>
   </si>
   <si>
     <t>fi</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>DRAFT</t>
-  </si>
-  <si>
-    <t/>
+    <t>Creative Commons Nimeä 4.0 Kansainvälinen (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons Erkännande 4.0 Internationell (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons Attribution 4.0 International (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Koodisto on lisensoitu Creative Commons Nimeä 4.0 Kansainvälinen -lisenssillä.</t>
   </si>
   <si>
     <t>Linkkikoodisto</t>
   </si>
   <si>
-    <t>2018-11-08 11:48:30</t>
+    <t>Detta kodelist är licensierat under en Creative Commons Erkännande 4.0 Internationell Licens.</t>
+  </si>
+  <si>
+    <t>testcode31</t>
+  </si>
+  <si>
+    <t>This code list is licensed under a Creative Commons Attribution 4.0 International License.</t>
+  </si>
+  <si>
+    <t>Testcode 31</t>
   </si>
   <si>
     <t>2018-11-08 11:52:52</t>
   </si>
   <si>
+    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
+  </si>
+  <si>
     <t>https://www.suomi.fi/etusivu/|test.com|test.fi|standardi.fi|https://creativecommons.org/licenses/by/4.0/|https://lähde.fi|testikäyttöohje.fi|https://creativecommons.org/publicdomain/zero/1.0/</t>
   </si>
   <si>
+    <t>Creative Commons CC0 1.0 Yleismaailmallinen (CC0 1.0)</t>
+  </si>
+  <si>
     <t>Codes_200</t>
   </si>
   <si>
-    <t>ExternalReferences_200</t>
+    <t>Creative Commons CC0 1.0 universell (CC0 1.0)</t>
+  </si>
+  <si>
+    <t>Links_200</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>Extensions_200</t>
   </si>
   <si>
-    <t>PROPERTYTYPE</t>
+    <t>Creative Commons CC0 1.0 Universal (CC0 1.0)</t>
+  </si>
+  <si>
+    <t>Koodisto on lisensoitu Creative Commons Zero (CC0) -lisenssillä.</t>
+  </si>
+  <si>
+    <t>Detta kodelist är licensierat under en Creative Commons Zero (CC0) Licens.</t>
+  </si>
+  <si>
+    <t>This code list is licensed under a Creative Commons Zero (CC0) License.</t>
+  </si>
+  <si>
+    <t>testcode32</t>
+  </si>
+  <si>
+    <t>Testcode 32</t>
+  </si>
+  <si>
+    <t>linkki.fi</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>testcode33</t>
+  </si>
+  <si>
+    <t>Testcode 33</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>testcode34</t>
+  </si>
+  <si>
+    <t>Testcode 34</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>testcode35</t>
+  </si>
+  <si>
+    <t>normilinkki</t>
+  </si>
+  <si>
+    <t>Testcode 35</t>
+  </si>
+  <si>
+    <t>normilinkki_sv</t>
+  </si>
+  <si>
+    <t>normilinkki_en</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>testcode36</t>
+  </si>
+  <si>
+    <t>Testcode 36</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>testcode37</t>
+  </si>
+  <si>
+    <t>Testcode 37</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>testcode38</t>
+  </si>
+  <si>
+    <t>Testcode 38</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>testcode39</t>
+  </si>
+  <si>
+    <t>Testcode 39</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>testcode40</t>
+  </si>
+  <si>
+    <t>Testcode 40</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>testcode41</t>
+  </si>
+  <si>
+    <t>Testcode 41</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>testcode42</t>
+  </si>
+  <si>
+    <t>Testcode 42</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>testcode43</t>
+  </si>
+  <si>
+    <t>Testcode 43</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>testcode44</t>
+  </si>
+  <si>
+    <t>Testcode 44</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>testcode45</t>
+  </si>
+  <si>
+    <t>Testcode 45</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>testcode46</t>
+  </si>
+  <si>
+    <t>Testcode 46</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>testcode47</t>
+  </si>
+  <si>
+    <t>Testcode 47</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>testcode48</t>
+  </si>
+  <si>
+    <t>Testcode 48</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>testcode49</t>
+  </si>
+  <si>
+    <t>Testcode 49</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>testcode50</t>
+  </si>
+  <si>
+    <t>Testcode 50</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>testcode51</t>
+  </si>
+  <si>
+    <t>Testcode 51</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>testcode52</t>
+  </si>
+  <si>
+    <t>Testcode 52</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>testcode53</t>
+  </si>
+  <si>
+    <t>Testcode 53</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>testcode54</t>
+  </si>
+  <si>
+    <t>Testcode 54</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>testcode55</t>
+  </si>
+  <si>
+    <t>Testcode 55</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>testcode56</t>
+  </si>
+  <si>
+    <t>Testcode 56</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>testcode57</t>
+  </si>
+  <si>
+    <t>Testcode 57</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>CODESCHEMES</t>
   </si>
   <si>
     <t>MEMBERSSHEET</t>
-  </si>
-  <si>
-    <t>TITLE_FI</t>
-  </si>
-  <si>
-    <t>TITLE_SV</t>
-  </si>
-  <si>
-    <t>BROADER</t>
-  </si>
-  <si>
-    <t>TITLE_EN</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
-  </si>
-  <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>HIERARCHYLEVEL</t>
-  </si>
-  <si>
-    <t>ORDER</t>
-  </si>
-  <si>
-    <t>https://lähde.fi</t>
-  </si>
-  <si>
-    <t>xxxx</t>
-  </si>
-  <si>
-    <t>Lähde</t>
-  </si>
-  <si>
-    <t>testcode28</t>
-  </si>
-  <si>
-    <t>Testcode 28</t>
-  </si>
-  <si>
-    <t>lähde.com</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>uusi lähde</t>
-  </si>
-  <si>
-    <t>2018-11-08 12:01:43</t>
-  </si>
-  <si>
-    <t>lisenssi.fi</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>uusi lisenssi</t>
-  </si>
-  <si>
-    <t>lähde.com|lisenssi.fi|käyttöohje.fi|linkki.fi</t>
-  </si>
-  <si>
-    <t>test.fi</t>
-  </si>
-  <si>
-    <t>isRequiredBy</t>
-  </si>
-  <si>
-    <t>käyttöedellytys</t>
-  </si>
-  <si>
-    <t>testcode29</t>
-  </si>
-  <si>
-    <t>https://www.suomi.fi/etusivu/</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>Testcode 29</t>
-  </si>
-  <si>
-    <t>test.com</t>
-  </si>
-  <si>
-    <t>isReferencedBy</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>käyttökohde</t>
-  </si>
-  <si>
-    <t>standardi.fi</t>
-  </si>
-  <si>
-    <t>lähde.com|lisenssi.fi</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
-    <t>Liittyvä standardi</t>
-  </si>
-  <si>
-    <t>testcode30</t>
-  </si>
-  <si>
-    <t>testikäyttöohje.fi</t>
-  </si>
-  <si>
-    <t>instructions</t>
-  </si>
-  <si>
-    <t>Käyttöohje</t>
-  </si>
-  <si>
-    <t>Testcode 30</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by/4.0/</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Creative Commons Nimeä 4.0 Kansainvälinen (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>Creative Commons Erkännande 4.0 Internationell (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>Creative Commons Attribution 4.0 International (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>Koodisto on lisensoitu Creative Commons Nimeä 4.0 Kansainvälinen -lisenssillä.</t>
-  </si>
-  <si>
-    <t>Detta kodelist är licensierat under en Creative Commons Erkännande 4.0 Internationell Licens.</t>
-  </si>
-  <si>
-    <t>This code list is licensed under a Creative Commons Attribution 4.0 International License.</t>
-  </si>
-  <si>
-    <t>testcode31</t>
-  </si>
-  <si>
-    <t>2018-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>Testcode 31</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
-  </si>
-  <si>
-    <t>Creative Commons CC0 1.0 Yleismaailmallinen (CC0 1.0)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Creative Commons CC0 1.0 universell (CC0 1.0)</t>
-  </si>
-  <si>
-    <t>Creative Commons CC0 1.0 Universal (CC0 1.0)</t>
-  </si>
-  <si>
-    <t>Koodisto on lisensoitu Creative Commons Zero (CC0) -lisenssillä.</t>
-  </si>
-  <si>
-    <t>Detta kodelist är licensierat under en Creative Commons Zero (CC0) Licens.</t>
-  </si>
-  <si>
-    <t>testcode32</t>
-  </si>
-  <si>
-    <t>This code list is licensed under a Creative Commons Zero (CC0) License.</t>
-  </si>
-  <si>
-    <t>Testcode 32</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>linkki.fi</t>
-  </si>
-  <si>
-    <t>testcode33</t>
-  </si>
-  <si>
-    <t>Testcode 33</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>testcode34</t>
-  </si>
-  <si>
-    <t>Testcode 34</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>testcode35</t>
-  </si>
-  <si>
-    <t>Testcode 35</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>testcode36</t>
-  </si>
-  <si>
-    <t>Testcode 36</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>testcode37</t>
-  </si>
-  <si>
-    <t>Testcode 37</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>testcode38</t>
-  </si>
-  <si>
-    <t>Testcode 38</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>testcode39</t>
-  </si>
-  <si>
-    <t>Testcode 39</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>testcode40</t>
-  </si>
-  <si>
-    <t>Testcode 40</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>normilinkki</t>
-  </si>
-  <si>
-    <t>normilinkki_sv</t>
-  </si>
-  <si>
-    <t>testcode41</t>
-  </si>
-  <si>
-    <t>normilinkki_en</t>
-  </si>
-  <si>
-    <t>Testcode 41</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>testcode42</t>
-  </si>
-  <si>
-    <t>Testcode 42</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>testcode43</t>
-  </si>
-  <si>
-    <t>Testcode 43</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>testcode44</t>
-  </si>
-  <si>
-    <t>Testcode 44</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>testcode45</t>
-  </si>
-  <si>
-    <t>Testcode 45</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>testcode46</t>
-  </si>
-  <si>
-    <t>Testcode 46</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>testcode47</t>
-  </si>
-  <si>
-    <t>Testcode 47</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>testcode48</t>
-  </si>
-  <si>
-    <t>Testcode 48</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>testcode49</t>
-  </si>
-  <si>
-    <t>Testcode 49</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>testcode50</t>
-  </si>
-  <si>
-    <t>Testcode 50</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>testcode51</t>
-  </si>
-  <si>
-    <t>Testcode 51</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>testcode52</t>
-  </si>
-  <si>
-    <t>Testcode 52</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>testcode53</t>
-  </si>
-  <si>
-    <t>Testcode 53</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>testcode54</t>
-  </si>
-  <si>
-    <t>Testcode 54</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>testcode55</t>
-  </si>
-  <si>
-    <t>Testcode 55</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>testcode56</t>
-  </si>
-  <si>
-    <t>Testcode 56</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>testcode57</t>
-  </si>
-  <si>
-    <t>Testcode 57</t>
-  </si>
-  <si>
-    <t>30</t>
   </si>
 </sst>
 </file>
@@ -593,9 +590,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -636,7 +631,9 @@
     <col customWidth="1" min="12" max="12" width="21.86"/>
     <col customWidth="1" min="13" max="16" width="8.71"/>
     <col customWidth="1" min="17" max="17" width="59.29"/>
-    <col customWidth="1" min="18" max="25" width="8.71"/>
+    <col customWidth="1" min="18" max="18" width="8.71"/>
+    <col customWidth="1" min="19" max="19" width="26.57"/>
+    <col customWidth="1" min="20" max="20" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -647,120 +644,120 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
       <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>200.0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>31</v>
+        <v>86</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1768,254 +1765,195 @@
     <col customWidth="1" min="5" max="5" width="21.57"/>
     <col customWidth="1" min="6" max="6" width="29.29"/>
     <col customWidth="1" min="7" max="7" width="8.71"/>
-    <col customWidth="1" min="8" max="8" width="30.43"/>
-    <col customWidth="1" min="9" max="25" width="8.71"/>
+    <col customWidth="1" min="8" max="8" width="19.71"/>
+    <col customWidth="1" min="9" max="9" width="29.0"/>
+    <col customWidth="1" min="10" max="10" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
         <v>91</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>129</v>
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3023,7 +2961,6 @@
     <col customWidth="1" min="11" max="11" width="23.29"/>
     <col customWidth="1" min="12" max="12" width="24.71"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
-    <col customWidth="1" min="14" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3031,368 +2968,368 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
         <v>89</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M6" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M7" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M8" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
         <v>110</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
@@ -3400,40 +3337,40 @@
         <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
         <v>113</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M10" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
@@ -3441,40 +3378,40 @@
         <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
         <v>116</v>
       </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M11" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -3482,40 +3419,40 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
         <v>119</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -3523,40 +3460,40 @@
         <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
         <v>122</v>
       </c>
       <c r="I13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M13" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -3564,737 +3501,737 @@
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
         <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
         <v>125</v>
       </c>
       <c r="I14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
         <v>128</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>131</v>
-      </c>
       <c r="I15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L15" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M15" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L16" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M16" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L17" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L18" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M18" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L19" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M19" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L20" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L21" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M21" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L22" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M22" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L23" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M23" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J24" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L24" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M24" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L25" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M25" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L26" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M26" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K27" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L27" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M27" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K28" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L28" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M28" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K29" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L29" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M29" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J30" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L30" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M30" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K31" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="L31" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="M31" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
@@ -5284,7 +5221,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="8.71"/>
+    <col customWidth="1" min="1" max="9" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5292,28 +5229,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>